<commit_message>
updates with new search rectangles and Chris' images
</commit_message>
<xml_diff>
--- a/ABBYY_Shootout.suite/Resources/ABBYY_IssueList.xlsx
+++ b/ABBYY_Shootout.suite/Resources/ABBYY_IssueList.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ScriptRepositories\ABBYY_Shootout\ABBYY_Shootout.suite\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C853C5-1C7A-46B1-B689-249A98017D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBCA6E5C-3753-4047-8920-7E50FF8277B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8850" yWindow="-21710" windowWidth="38620" windowHeight="21100"/>
+    <workbookView xWindow="1480" yWindow="1480" windowWidth="28800" windowHeight="15360"/>
   </bookViews>
   <sheets>
-    <sheet name="Last 24 hours Failed Scheduled " sheetId="1" r:id="rId1"/>
+    <sheet name="Original" sheetId="1" r:id="rId1"/>
+    <sheet name="Extra Crispy" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" fullCalcOnLoad="true" refMode="R1C1"/>
+  <calcPr calcId="0" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="28" uniqueCount="22">
   <si>
     <t>Script</t>
   </si>
@@ -62,6 +63,30 @@
   </si>
   <si>
     <t>RecNumber</t>
+  </si>
+  <si>
+    <t>Imagefound(text:"Episode", SearchRectangle: [231,209,1896,247], waitFor: 1)</t>
+  </si>
+  <si>
+    <t>Imagefound(TEXT:"Application Access Menu", validWords:"*")</t>
+  </si>
+  <si>
+    <t>Imagefound(TEXT:"ZZZeggplant, IPInfection",ValidCharacters:"A".."Z" &amp;&amp;&amp; "a".."z" &amp;&amp;&amp; "," &amp;&amp;&amp; ".",IgnoreSpaces:yes,waitfor:0,textDifference:1,ignorenewlines:yes ,searchRectangle:[465,194,573,1078])</t>
+  </si>
+  <si>
+    <t>Imagefound(TEXT:"ZZZeggplant, IPwardnurse",ValidCharacters:"A".."Z" &amp;&amp;&amp; "a".."z" &amp;&amp;&amp; "," &amp;&amp;&amp; ".",IgnoreSpaces:yes,waitfor:0,textDifference:1,ignorenewlines:yes ,searchRectangle:[465,194,573,1078])</t>
+  </si>
+  <si>
+    <t>Imagefound(text:"In", waitFor:0,caseSensitive:"yes", SearchRectangle: [655,347,1265,652])</t>
+  </si>
+  <si>
+    <t>imageFound(text: "patient", searchRectangle:[1240,143,1915,1034])</t>
+  </si>
+  <si>
+    <t>imageFound(dpi:"144", SearchRectangle:[230,240,1919,279], text:"Hide Add'l Visits", TextDifference:"2")</t>
+  </si>
+  <si>
+    <t>Imagefound(SearchRectangle:[435,155,1482,972], text:"Arrange Views")</t>
   </si>
 </sst>
 </file>
@@ -956,21 +981,204 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEDF119E-664B-4170-8994-2CAC0F6CD390}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="true" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11" style="5" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="14.36328125" style="5" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="168.81640625" style="7" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="11.6328125" style="7" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="12.08984375" style="2" bestFit="true" customWidth="true"/>
+    <col min="6" max="6" width="12.6328125" style="2" bestFit="true" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.35">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5">
+        <v>63223</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="6">
+        <v>12.2</v>
+      </c>
+      <c r="E2" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.35">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5">
+        <v>63253</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="6">
+        <v>12.2</v>
+      </c>
+      <c r="E3" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.35">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5">
+        <v>63262</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="6">
+        <v>12.2</v>
+      </c>
+      <c r="E4" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.35">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5">
+        <v>63246</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="6">
+        <v>12.2</v>
+      </c>
+      <c r="E5" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.35">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5">
+        <v>63222</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="6">
+        <v>12.2</v>
+      </c>
+      <c r="E6" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.35">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5">
+        <v>63130</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="6">
+        <v>12.2</v>
+      </c>
+      <c r="E7" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.35">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5">
+        <v>63190</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="6">
+        <v>12.2</v>
+      </c>
+      <c r="E8" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.35">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5">
+        <v>63090</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="6">
+        <v>12.4</v>
+      </c>
+      <c r="E9" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" x14ac:dyDescent="0.35">
+      <c r="C10" s="8"/>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="13" x14ac:dyDescent="0.35">
+      <c r="D13" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18B94BF2-A15F-4905-9619-72031F4A7DBC}">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E2:E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11" style="5" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="14.33203125" style="5" bestFit="true" customWidth="true"/>
-    <col min="3" max="3" width="168.77734375" style="7" bestFit="true" customWidth="true"/>
-    <col min="4" max="4" width="11.6640625" style="7" bestFit="true" customWidth="true"/>
-    <col min="5" max="5" width="12.109375" style="2" bestFit="true" customWidth="true"/>
-    <col min="6" max="6" width="12.6640625" style="2" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="14.36328125" style="5" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="168.81640625" style="7" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="11.6328125" style="7" bestFit="true" customWidth="true"/>
+    <col min="5" max="5" width="12.08984375" style="2" bestFit="true" customWidth="true"/>
+    <col min="6" max="6" width="12.6328125" style="2" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" x14ac:dyDescent="0.3">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
@@ -990,7 +1198,7 @@
         <v>4</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.3">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="2" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -998,7 +1206,7 @@
         <v>63223</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D2" s="6">
         <v>12.2</v>
@@ -1007,7 +1215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.3">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="3" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1015,7 +1223,7 @@
         <v>63253</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D3" s="6">
         <v>12.2</v>
@@ -1024,7 +1232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.3">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="4" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1032,7 +1240,7 @@
         <v>63262</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D4" s="6">
         <v>12.2</v>
@@ -1041,7 +1249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.3">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="5" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1049,7 +1257,7 @@
         <v>63246</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D5" s="6">
         <v>12.2</v>
@@ -1058,7 +1266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.3">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="6" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1066,7 +1274,7 @@
         <v>63222</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D6" s="6">
         <v>12.2</v>
@@ -1075,7 +1283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.3">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="7" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1083,7 +1291,7 @@
         <v>63130</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D7" s="6">
         <v>12.2</v>
@@ -1092,7 +1300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.3">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="8" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1100,7 +1308,7 @@
         <v>63190</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D8" s="6">
         <v>12.2</v>
@@ -1109,7 +1317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.3">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="9" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1117,19 +1325,19 @@
         <v>63090</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="D9" s="6">
         <v>12.4</v>
       </c>
       <c r="E9" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="10" x14ac:dyDescent="0.35">
       <c r="C10" s="8"/>
     </row>
-    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="13" x14ac:dyDescent="0.3">
+    <row xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" r="13" x14ac:dyDescent="0.35">
       <c r="D13" s="8"/>
     </row>
   </sheetData>

</xml_diff>